<commit_message>
Fixed conveying blocks so that they evenly move the player (however this fix was only done for horizontal movement).
</commit_message>
<xml_diff>
--- a/Platformer/Color Converter.xlsx
+++ b/Platformer/Color Converter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="1280" windowWidth="15200" windowHeight="7580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,114 +350,114 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="B1">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="C1">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D1">
         <f t="shared" ref="D1:F4" si="0">A1/255</f>
-        <v>0.21176470588235294</v>
+        <v>0</v>
       </c>
       <c r="E1">
         <f t="shared" si="0"/>
-        <v>0.23921568627450981</v>
+        <v>2.7450980392156862E-2</v>
       </c>
       <c r="F1">
         <f t="shared" si="0"/>
-        <v>0.44705882352941179</v>
+        <v>0.45882352941176469</v>
       </c>
       <c r="G1" t="str">
         <f>"Color(r: "&amp;TEXT(D1,"0.000")&amp;", g: "&amp;TEXT(E1,"0.000")&amp;", b: "&amp;TEXT(F1,"0.000")&amp;", a: 1)"</f>
-        <v>Color(r: 0.212, g: 0.239, b: 0.447, a: 1)</v>
+        <v>Color(r: 0.000, g: 0.027, b: 0.459, a: 1)</v>
       </c>
       <c r="H1" t="str">
         <f>"gameScene.setColor("&amp;TEXT(G1,"")&amp;", "&amp;TEXT(G2,"")&amp;", "&amp;TEXT(G3,"")&amp;", "&amp;TEXT(G4,"")&amp;")"</f>
-        <v>gameScene.setColor(Color(r: 0.212, g: 0.239, b: 0.447, a: 1), Color(r: 0.400, g: 0.231, b: 0.525, a: 1), Color(r: 0.894, g: 0.310, b: 0.545, a: 1), Color(r: 0.776, g: 0.620, b: 0.839, a: 1))</v>
+        <v>gameScene.setColor(Color(r: 0.000, g: 0.027, b: 0.459, a: 1), Color(r: 0.984, g: 0.082, b: 0.486, a: 1), Color(r: 0.996, g: 0.992, b: 0.498, a: 1), Color(r: 0.165, g: 0.992, b: 0.478, a: 1))</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>102</v>
+        <v>251</v>
       </c>
       <c r="B2">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="C2">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D2">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.98431372549019602</v>
       </c>
       <c r="E2">
         <f t="shared" si="0"/>
-        <v>0.23137254901960785</v>
+        <v>8.2352941176470587E-2</v>
       </c>
       <c r="F2">
         <f t="shared" si="0"/>
-        <v>0.52549019607843139</v>
+        <v>0.48627450980392156</v>
       </c>
       <c r="G2" t="str">
         <f>"Color(r: "&amp;TEXT(D2,"0.000")&amp;", g: "&amp;TEXT(E2,"0.000")&amp;", b: "&amp;TEXT(F2,"0.000")&amp;", a: 1)"</f>
-        <v>Color(r: 0.400, g: 0.231, b: 0.525, a: 1)</v>
+        <v>Color(r: 0.984, g: 0.082, b: 0.486, a: 1)</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="B3">
-        <v>79</v>
+        <v>253</v>
       </c>
       <c r="C3">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>0.89411764705882357</v>
+        <v>0.99607843137254903</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>0.30980392156862746</v>
+        <v>0.99215686274509807</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>0.54509803921568623</v>
+        <v>0.49803921568627452</v>
       </c>
       <c r="G3" t="str">
         <f>"Color(r: "&amp;TEXT(D3,"0.000")&amp;", g: "&amp;TEXT(E3,"0.000")&amp;", b: "&amp;TEXT(F3,"0.000")&amp;", a: 1)"</f>
-        <v>Color(r: 0.894, g: 0.310, b: 0.545, a: 1)</v>
+        <v>Color(r: 0.996, g: 0.992, b: 0.498, a: 1)</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>198</v>
+        <v>42</v>
       </c>
       <c r="B4">
-        <v>158</v>
+        <v>253</v>
       </c>
       <c r="C4">
-        <v>214</v>
+        <v>122</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0.77647058823529413</v>
+        <v>0.16470588235294117</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0.61960784313725492</v>
+        <v>0.99215686274509807</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0.83921568627450982</v>
+        <v>0.47843137254901963</v>
       </c>
       <c r="G4" t="str">
         <f>"Color(r: "&amp;TEXT(D4,"0.000")&amp;", g: "&amp;TEXT(E4,"0.000")&amp;", b: "&amp;TEXT(F4,"0.000")&amp;", a: 1)"</f>
-        <v>Color(r: 0.776, g: 0.620, b: 0.839, a: 1)</v>
+        <v>Color(r: 0.165, g: 0.992, b: 0.478, a: 1)</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>